<commit_message>
feat: use html template for transcript exporting
</commit_message>
<xml_diff>
--- a/backend/src/main/resources/templates/template.xlsx
+++ b/backend/src/main/resources/templates/template.xlsx
@@ -68,6 +68,19 @@
         </r>
       </text>
     </comment>
+    <comment ref="A15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Liberation Mono;Courier New;Cousine;DejaVu Sans Mono;Lucida Sans Typewriter"/>
+            <family val="3"/>
+          </rPr>
+          <t xml:space="preserve">jx:area(lastCell="G100") 
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -117,7 +130,7 @@
     <t xml:space="preserve">B</t>
   </si>
   <si>
-    <t xml:space="preserve">v.2.7</t>
+    <t xml:space="preserve">v.2.8</t>
   </si>
   <si>
     <t xml:space="preserve">Header D</t>
@@ -148,7 +161,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -205,6 +218,11 @@
       <sz val="10"/>
       <name val="JetBrains Mono"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Liberation Mono;Courier New;Cousine;DejaVu Sans Mono;Lucida Sans Typewriter"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -444,10 +462,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -578,26 +596,56 @@
       <c r="G12" s="1"/>
       <c r="H12" s="0"/>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+    <row r="13" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="0"/>
+    </row>
+    <row r="14" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="0"/>
+    </row>
+    <row r="15" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B16" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="15"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F18" s="3" t="s">
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="15"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F21" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="3"/>
+      <c r="G21" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -615,8 +663,8 @@
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F21:G21"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>